<commit_message>
committing rmd and new metadata
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Dropbox (Personal)\nes-lter-npp-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07C3297-6140-44F1-AFBF-F39718030BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572FA7EB-DCF5-4322-8249-43668B3BCAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28812" yWindow="-3768" windowWidth="24108" windowHeight="9108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31590" yWindow="9435" windowWidth="21600" windowHeight="7560" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,27 @@
     <sheet name="Keywords" sheetId="5" r:id="rId5"/>
     <sheet name="CustomUnits" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="165">
   <si>
     <t>attributeName</t>
   </si>
@@ -386,9 +396,6 @@
     <t>Integer indicating replicate subsample drawn from the same Niskin</t>
   </si>
   <si>
-    <t>miligramPerMeterSquaredPerDay</t>
-  </si>
-  <si>
     <t>stable isotopes</t>
   </si>
   <si>
@@ -422,31 +429,112 @@
     <t>A</t>
   </si>
   <si>
-    <t>Cast occurred at night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cast occurred during daylight </t>
-  </si>
-  <si>
-    <t>Deepest samples</t>
-  </si>
-  <si>
-    <t>Shallowest samples</t>
-  </si>
-  <si>
-    <t>Category describing where in water column sample was obtained</t>
-  </si>
-  <si>
     <t>Identifer combining filter size with other information</t>
   </si>
   <si>
-    <t>Calculated from depth and light extinction coefficient for each station</t>
-  </si>
-  <si>
-    <t>Calculated based on equation from Hama et al 1983</t>
-  </si>
-  <si>
     <t>microgramPerLiterPerDay</t>
+  </si>
+  <si>
+    <t>Net primary productivity in micrograms carbon per liter per day determined by uptake rate of labeled bicarbonate</t>
+  </si>
+  <si>
+    <t>Vertically-integrated net primary productivity measured as uptake rate of carbon per unit area of water per day</t>
+  </si>
+  <si>
+    <t>Category based on light extinction that describes where in water column sample was obtained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deepest depth sampled based on light extinction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cast occurred during daylight </t>
+  </si>
+  <si>
+    <t>cast occurred at night</t>
+  </si>
+  <si>
+    <t>second-deepest depth sampled based on light extinction</t>
+  </si>
+  <si>
+    <t>where three depths are sampled at a station, the category for shallowest samples; where four depths are sampled, the category for second-shallowest samples</t>
+  </si>
+  <si>
+    <t>where four depths are sampled at a station, the category for the shallowest samples</t>
+  </si>
+  <si>
+    <t>0.1 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>1 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>5 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>10 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>15 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>20 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>30 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>40 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>50 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>65 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>70 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>75 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>85percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>milligramPerMeterSquaredPerDay</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>samples collected from dark amber bottles to observe any light-independent carbon fixation</t>
+  </si>
+  <si>
+    <t>Light at sample location as a percent of surface photosynthetically active radiation (PAR), calculated based on light extinction coefficient for each station</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>Meter</t>
+  </si>
+  <si>
+    <t>attenuation rate</t>
+  </si>
+  <si>
+    <t>volumetricMassDensityRate</t>
+  </si>
+  <si>
+    <t>micrograms per liter per day</t>
+  </si>
+  <si>
+    <t>1^-1</t>
+  </si>
+  <si>
+    <t>gramPerDayPerLiter</t>
+  </si>
+  <si>
+    <t>1e-06</t>
   </si>
 </sst>
 </file>
@@ -483,18 +571,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -531,9 +613,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -817,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,8 +1076,8 @@
       <c r="A9" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>135</v>
+      <c r="B9" s="10" t="s">
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -1005,8 +1087,8 @@
       <c r="A10" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>134</v>
+      <c r="B10" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>91</v>
@@ -1030,25 +1112,28 @@
       <c r="B12" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
       <c r="F12" t="s">
         <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="10"/>
       <c r="F13" t="s">
         <v>10</v>
       </c>
@@ -1060,14 +1145,14 @@
       <c r="A14" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>137</v>
+      <c r="B14" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>138</v>
+      <c r="D14" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -1086,7 +1171,7 @@
       <c r="C15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="10"/>
       <c r="F15" t="s">
         <v>10</v>
       </c>
@@ -1142,7 +1227,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A12" sqref="A12:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,8 +1353,12 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1307,12 +1396,14 @@
       <c r="A9" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1330,8 +1421,8 @@
       <c r="A11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>125</v>
+      <c r="B11" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
@@ -1341,42 +1432,60 @@
       <c r="A12" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>123</v>
+      <c r="B12" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>124</v>
+      <c r="D12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>126</v>
+      <c r="B13" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>124</v>
+      <c r="D13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>127</v>
+      <c r="B14" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>124</v>
+      <c r="D14" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1387,9 +1496,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCA061C-6977-48E5-9053-BCD9FB4DDE1B}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1436,7 +1545,7 @@
         <v>79</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
         <v>115</v>
@@ -1504,8 +1613,8 @@
       <c r="B10" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>131</v>
+      <c r="C10" s="10" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1515,8 +1624,8 @@
       <c r="B11" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>130</v>
+      <c r="C11" s="10" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1524,10 +1633,10 @@
         <v>78</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>132</v>
+        <v>154</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1535,158 +1644,203 @@
         <v>78</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>109</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="10"/>
+        <v>110</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16">
-        <v>0.1</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>81</v>
       </c>
       <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>81</v>
       </c>
       <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
       <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>81</v>
       </c>
       <c r="B20">
-        <v>15</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
       <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>81</v>
       </c>
       <c r="B22">
-        <v>30</v>
-      </c>
-      <c r="C22" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>81</v>
       </c>
       <c r="B23">
-        <v>40</v>
-      </c>
-      <c r="C23" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
       <c r="B24">
-        <v>50</v>
-      </c>
-      <c r="C24" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>81</v>
       </c>
       <c r="B25">
-        <v>65</v>
-      </c>
-      <c r="C25" s="10"/>
+        <v>50</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>81</v>
       </c>
       <c r="B26">
-        <v>70</v>
-      </c>
-      <c r="C26" s="10"/>
+        <v>65</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
       <c r="B27">
-        <v>75</v>
-      </c>
-      <c r="C27" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>81</v>
       </c>
       <c r="B28">
+        <v>75</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29">
         <v>85</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C29" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FB71B2-251C-4C70-A42B-DE90E8FB59EC}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,7 +1887,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
@@ -1760,24 +1914,24 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>108</v>
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
         <v>61</v>
@@ -1796,7 +1950,7 @@
       <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>108</v>
       </c>
       <c r="C4" t="s">
@@ -1812,7 +1966,7 @@
         <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
         <v>58</v>
@@ -1826,13 +1980,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="E5" t="s">
-        <v>70</v>
+      <c r="E5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
       </c>
       <c r="G5" t="s">
         <v>71</v>
@@ -1849,22 +2012,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" t="s">
-        <v>76</v>
+      <c r="E6" t="s">
+        <v>70</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" t="s">
         <v>58</v>
@@ -1873,15 +2030,45 @@
         <v>62</v>
       </c>
       <c r="J6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{B876B57E-F40C-4019-9902-E3F5F210A4B5}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{BC3EDBC0-671D-451E-BB61-743090D6124F}"/>
-    <hyperlink ref="E6" r:id="rId3" xr:uid="{ABC8AAB7-95D6-4B09-8D74-EC58F97B7FC9}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{B197A09B-50AF-4335-9439-0ADC5614820A}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{BC3EDBC0-671D-451E-BB61-743090D6124F}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{ABC8AAB7-95D6-4B09-8D74-EC58F97B7FC9}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{B197A09B-50AF-4335-9439-0ADC5614820A}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{C478F55C-B590-48E5-AECF-BCE8DA56F3E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1943,7 +2130,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -1951,7 +2138,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
@@ -1959,7 +2146,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -1967,7 +2154,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -1988,13 +2175,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B88C0FB-B81B-4182-8D44-742C6584AC87}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="55.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2013,7 +2204,45 @@
         <v>47</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated a col name and daytime_Y_N defn
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58DCF40-5D58-41D1-A3C1-86C369A81714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F12E1BB-287A-4D88-87FF-DF3DB1B12D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28860" yWindow="9420" windowWidth="28305" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29265" yWindow="6465" windowWidth="28305" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
@@ -273,9 +273,6 @@
     <t>0000-0002-2903-5851</t>
   </si>
   <si>
-    <t>alternate_sample_ID</t>
-  </si>
-  <si>
     <t>depth_category</t>
   </si>
   <si>
@@ -414,9 +411,6 @@
     <t>perMeter</t>
   </si>
   <si>
-    <t>Designation for whether cast occurred during day or night</t>
-  </si>
-  <si>
     <t>Average beam attenuation (At) measured by ship's transmissometer within the upper 10 m of  water column</t>
   </si>
   <si>
@@ -535,6 +529,12 @@
   </si>
   <si>
     <t>85 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>alternate_sample_category</t>
+  </si>
+  <si>
+    <t>Casts with surface PAR above 10 micromol photons/m/s classified as daytime</t>
   </si>
 </sst>
 </file>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,10 +1074,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -1085,32 +1085,32 @@
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>9</v>
@@ -1125,13 +1125,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="10"/>
       <c r="F13" t="s">
@@ -1143,16 +1143,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -1163,13 +1163,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="10"/>
       <c r="F15" t="s">
@@ -1181,10 +1181,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -1193,27 +1193,27 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1227,7 +1227,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,7 +1346,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -1383,63 +1383,63 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>10</v>
@@ -1450,16 +1450,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>10</v>
@@ -1470,16 +1470,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>10</v>
@@ -1520,310 +1520,310 @@
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
         <v>113</v>
-      </c>
-      <c r="C3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="7">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="7">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17">
         <v>0.1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21">
         <v>15</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23">
         <v>30</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24">
         <v>40</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25">
         <v>50</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26">
         <v>65</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27">
         <v>70</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28">
         <v>75</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29">
         <v>85</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1887,7 +1887,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
@@ -1919,7 +1919,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>57</v>
@@ -1951,7 +1951,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
         <v>65</v>
@@ -1983,7 +1983,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -2154,7 +2154,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -2206,36 +2206,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
         <v>156</v>
-      </c>
-      <c r="C2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Pierre, light, rapid parent proj, edit methods
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F12E1BB-287A-4D88-87FF-DF3DB1B12D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DEE49-67FC-4CB5-B825-8F37EFF5FB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29265" yWindow="6465" windowWidth="28305" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26595" yWindow="1935" windowWidth="28470" windowHeight="12900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="169">
   <si>
     <t>attributeName</t>
   </si>
@@ -258,283 +258,295 @@
     <t>contact</t>
   </si>
   <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Morkeski</t>
+  </si>
+  <si>
+    <t>kmorkeski@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0002-2903-5851</t>
+  </si>
+  <si>
+    <t>depth_category</t>
+  </si>
+  <si>
+    <t>filter_size</t>
+  </si>
+  <si>
+    <t>replicate</t>
+  </si>
+  <si>
+    <t>percent_surface_irradiance</t>
+  </si>
+  <si>
+    <t>npp_rate</t>
+  </si>
+  <si>
+    <t>iode_quality_flag</t>
+  </si>
+  <si>
+    <t>nearest_station</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>integrated_npp_mg_m2_day</t>
+  </si>
+  <si>
+    <t>daytime_Y_N</t>
+  </si>
+  <si>
+    <t>k_meas_per_m</t>
+  </si>
+  <si>
+    <t>beam_atten_0_10</t>
+  </si>
+  <si>
+    <t>k_calc_per_m</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size fraction with filter and when applicable prefilter pore size in micrometers </t>
+  </si>
+  <si>
+    <t>IODE Quality Flag primary level</t>
+  </si>
+  <si>
+    <t>&gt;0</t>
+  </si>
+  <si>
+    <t>Filtered on 0.7 micron filter</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>quality not evaluated, not available or unknown</t>
+  </si>
+  <si>
+    <t>questionable/suspect</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>missing data</t>
+  </si>
+  <si>
+    <t>NES-LTER standard station nearest to the sample location</t>
+  </si>
+  <si>
+    <t>Distance greater than 2 km from NES-LTER standard station</t>
+  </si>
+  <si>
+    <t>Distance from sample location to nearest NES-LTER standard station</t>
+  </si>
+  <si>
+    <t>kilometer</t>
+  </si>
+  <si>
+    <t>oceanography</t>
+  </si>
+  <si>
+    <t>seawater</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;0&amp;&lt;20 </t>
+  </si>
+  <si>
+    <t>Filtered on 0.7 micron filter with 20 micron prefilter</t>
+  </si>
+  <si>
+    <t>Filtered on 0.7 micron filter with 5 micron prefilter</t>
+  </si>
+  <si>
+    <t>NES-LTER standard station from which sample was collected</t>
+  </si>
+  <si>
+    <t>Integer indicating replicate subsample drawn from the same Niskin</t>
+  </si>
+  <si>
+    <t>stable isotopes</t>
+  </si>
+  <si>
+    <t>tracers</t>
+  </si>
+  <si>
+    <t>phytoplankton</t>
+  </si>
+  <si>
+    <t>particulate organic carbon</t>
+  </si>
+  <si>
+    <t>Measured light extinction coefficient</t>
+  </si>
+  <si>
+    <t>perMeter</t>
+  </si>
+  <si>
+    <t>Light extinction coefficient calculated from the measured daytime light extinction coefficient and beam attenuation</t>
+  </si>
+  <si>
+    <t>&gt;0&amp;&lt;5</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Identifer combining filter size with other information</t>
+  </si>
+  <si>
+    <t>microgramPerLiterPerDay</t>
+  </si>
+  <si>
+    <t>Net primary productivity in micrograms carbon per liter per day determined by uptake rate of labeled bicarbonate</t>
+  </si>
+  <si>
+    <t>Vertically-integrated net primary productivity measured as uptake rate of carbon per unit area of water per day</t>
+  </si>
+  <si>
+    <t>Category based on light extinction that describes where in water column sample was obtained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deepest depth sampled based on light extinction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cast occurred during daylight </t>
+  </si>
+  <si>
+    <t>cast occurred at night</t>
+  </si>
+  <si>
+    <t>second-deepest depth sampled based on light extinction</t>
+  </si>
+  <si>
+    <t>where three depths are sampled at a station, the category for shallowest samples; where four depths are sampled, the category for second-shallowest samples</t>
+  </si>
+  <si>
+    <t>where four depths are sampled at a station, the category for the shallowest samples</t>
+  </si>
+  <si>
+    <t>0.1 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>1 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>5 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>10 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>15 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>20 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>30 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>40 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>50 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>65 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>70 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>75 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>milligramPerMeterSquaredPerDay</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>samples collected from dark amber bottles to observe any light-independent carbon fixation</t>
+  </si>
+  <si>
+    <t>Light at sample location as a percent of surface photosynthetically active radiation (PAR), calculated based on light extinction coefficient for each station</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>Meter</t>
+  </si>
+  <si>
+    <t>attenuation rate</t>
+  </si>
+  <si>
+    <t>volumetricMassDensityRate</t>
+  </si>
+  <si>
+    <t>micrograms per liter per day</t>
+  </si>
+  <si>
+    <t>1^-1</t>
+  </si>
+  <si>
+    <t>gramPerDayPerLiter</t>
+  </si>
+  <si>
+    <t>1e-06</t>
+  </si>
+  <si>
+    <t>85 percent surface photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>alternate_sample_category</t>
+  </si>
+  <si>
+    <t>Casts with surface PAR above 10 micromol photons/m/s classified as daytime</t>
+  </si>
+  <si>
+    <t>Average beam attenuation (At) measured by ship's transmissometer within the upper 10 m of water column</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Marrec</t>
+  </si>
+  <si>
+    <t>pmarrec@uri.edu</t>
+  </si>
+  <si>
+    <t>0000-0002-7811-4150</t>
+  </si>
+  <si>
     <t>metadata Provider</t>
-  </si>
-  <si>
-    <t>Kate</t>
-  </si>
-  <si>
-    <t>Morkeski</t>
-  </si>
-  <si>
-    <t>kmorkeski@whoi.edu</t>
-  </si>
-  <si>
-    <t>0000-0002-2903-5851</t>
-  </si>
-  <si>
-    <t>depth_category</t>
-  </si>
-  <si>
-    <t>filter_size</t>
-  </si>
-  <si>
-    <t>replicate</t>
-  </si>
-  <si>
-    <t>percent_surface_irradiance</t>
-  </si>
-  <si>
-    <t>npp_rate</t>
-  </si>
-  <si>
-    <t>iode_quality_flag</t>
-  </si>
-  <si>
-    <t>nearest_station</t>
-  </si>
-  <si>
-    <t>distance</t>
-  </si>
-  <si>
-    <t>integrated_npp_mg_m2_day</t>
-  </si>
-  <si>
-    <t>daytime_Y_N</t>
-  </si>
-  <si>
-    <t>k_meas_per_m</t>
-  </si>
-  <si>
-    <t>beam_atten_0_10</t>
-  </si>
-  <si>
-    <t>k_calc_per_m</t>
-  </si>
-  <si>
-    <t>categorical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Size fraction with filter and when applicable prefilter pore size in micrometers </t>
-  </si>
-  <si>
-    <t>IODE Quality Flag primary level</t>
-  </si>
-  <si>
-    <t>&gt;0</t>
-  </si>
-  <si>
-    <t>Filtered on 0.7 micron filter</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>quality not evaluated, not available or unknown</t>
-  </si>
-  <si>
-    <t>questionable/suspect</t>
-  </si>
-  <si>
-    <t>bad</t>
-  </si>
-  <si>
-    <t>missing data</t>
-  </si>
-  <si>
-    <t>NES-LTER standard station nearest to the sample location</t>
-  </si>
-  <si>
-    <t>Distance greater than 2 km from NES-LTER standard station</t>
-  </si>
-  <si>
-    <t>Distance from sample location to nearest NES-LTER standard station</t>
-  </si>
-  <si>
-    <t>kilometer</t>
-  </si>
-  <si>
-    <t>oceanography</t>
-  </si>
-  <si>
-    <t>seawater</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;0&amp;&lt;20 </t>
-  </si>
-  <si>
-    <t>Filtered on 0.7 micron filter with 20 micron prefilter</t>
-  </si>
-  <si>
-    <t>Filtered on 0.7 micron filter with 5 micron prefilter</t>
-  </si>
-  <si>
-    <t>NES-LTER standard station from which sample was collected</t>
-  </si>
-  <si>
-    <t>Integer indicating replicate subsample drawn from the same Niskin</t>
-  </si>
-  <si>
-    <t>stable isotopes</t>
-  </si>
-  <si>
-    <t>tracers</t>
-  </si>
-  <si>
-    <t>phytoplankton</t>
-  </si>
-  <si>
-    <t>particulate organic carbon</t>
-  </si>
-  <si>
-    <t>Measured light extinction coefficient</t>
-  </si>
-  <si>
-    <t>perMeter</t>
-  </si>
-  <si>
-    <t>Average beam attenuation (At) measured by ship's transmissometer within the upper 10 m of  water column</t>
-  </si>
-  <si>
-    <t>Light extinction coefficient calculated from the measured daytime light extinction coefficient and beam attenuation</t>
-  </si>
-  <si>
-    <t>&gt;0&amp;&lt;5</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Identifer combining filter size with other information</t>
-  </si>
-  <si>
-    <t>microgramPerLiterPerDay</t>
-  </si>
-  <si>
-    <t>Net primary productivity in micrograms carbon per liter per day determined by uptake rate of labeled bicarbonate</t>
-  </si>
-  <si>
-    <t>Vertically-integrated net primary productivity measured as uptake rate of carbon per unit area of water per day</t>
-  </si>
-  <si>
-    <t>Category based on light extinction that describes where in water column sample was obtained</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deepest depth sampled based on light extinction </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cast occurred during daylight </t>
-  </si>
-  <si>
-    <t>cast occurred at night</t>
-  </si>
-  <si>
-    <t>second-deepest depth sampled based on light extinction</t>
-  </si>
-  <si>
-    <t>where three depths are sampled at a station, the category for shallowest samples; where four depths are sampled, the category for second-shallowest samples</t>
-  </si>
-  <si>
-    <t>where four depths are sampled at a station, the category for the shallowest samples</t>
-  </si>
-  <si>
-    <t>0.1 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>1 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>5 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>10 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>15 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>20 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>30 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>40 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>50 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>65 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>70 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>75 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>milligramPerMeterSquaredPerDay</t>
-  </si>
-  <si>
-    <t>Dark</t>
-  </si>
-  <si>
-    <t>samples collected from dark amber bottles to observe any light-independent carbon fixation</t>
-  </si>
-  <si>
-    <t>Light at sample location as a percent of surface photosynthetically active radiation (PAR), calculated based on light extinction coefficient for each station</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>Meter</t>
-  </si>
-  <si>
-    <t>attenuation rate</t>
-  </si>
-  <si>
-    <t>volumetricMassDensityRate</t>
-  </si>
-  <si>
-    <t>micrograms per liter per day</t>
-  </si>
-  <si>
-    <t>1^-1</t>
-  </si>
-  <si>
-    <t>gramPerDayPerLiter</t>
-  </si>
-  <si>
-    <t>1e-06</t>
-  </si>
-  <si>
-    <t>85 percent surface photosynthetically active radiation</t>
-  </si>
-  <si>
-    <t>alternate_sample_category</t>
-  </si>
-  <si>
-    <t>Casts with surface PAR above 10 micromol photons/m/s classified as daytime</t>
   </si>
 </sst>
 </file>
@@ -899,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1074,10 +1086,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -1085,32 +1097,32 @@
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>9</v>
@@ -1125,13 +1137,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="10"/>
       <c r="F13" t="s">
@@ -1143,16 +1155,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -1163,13 +1175,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="10"/>
       <c r="F15" t="s">
@@ -1181,10 +1193,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -1193,27 +1205,27 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1346,7 +1358,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -1383,63 +1395,63 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>10</v>
@@ -1450,16 +1462,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>10</v>
@@ -1470,16 +1482,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>10</v>
@@ -1520,310 +1532,310 @@
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="7">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="7">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17">
         <v>0.1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21">
         <v>15</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23">
         <v>30</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24">
         <v>40</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25">
         <v>50</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26">
         <v>65</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27">
         <v>70</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28">
         <v>75</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29">
         <v>85</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1837,10 +1849,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FB71B2-251C-4C70-A42B-DE90E8FB59EC}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1887,7 +1899,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
@@ -1919,7 +1931,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
         <v>57</v>
@@ -1951,7 +1963,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>65</v>
@@ -1983,7 +1995,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
@@ -2035,22 +2047,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
         <v>73</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
         <v>75</v>
       </c>
-      <c r="F7" t="s">
-        <v>76</v>
-      </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>168</v>
       </c>
       <c r="H7" t="s">
         <v>58</v>
@@ -2059,6 +2071,35 @@
         <v>62</v>
       </c>
       <c r="J7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2069,6 +2110,7 @@
     <hyperlink ref="E7" r:id="rId3" xr:uid="{ABC8AAB7-95D6-4B09-8D74-EC58F97B7FC9}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{B197A09B-50AF-4335-9439-0ADC5614820A}"/>
     <hyperlink ref="E3" r:id="rId5" xr:uid="{C478F55C-B590-48E5-AECF-BCE8DA56F3E8}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{46C996E6-62E0-4AE9-860A-E9CECA7008F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2114,7 +2156,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2122,7 +2164,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -2130,7 +2172,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -2138,7 +2180,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
@@ -2146,7 +2188,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -2154,7 +2196,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -2206,36 +2248,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" t="s">
         <v>154</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated methods and integrated defns
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1A345B-3287-45B3-AADE-113DB8487EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7576A145-E6FF-428B-821E-B52D0B9EC6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="172">
   <si>
     <t>attributeName</t>
   </si>
@@ -547,6 +547,15 @@
   </si>
   <si>
     <t>Category describing light at sample location as a percent of surface photosynthetically active radiation (PAR), calculated based on light extinction coefficient for each station</t>
+  </si>
+  <si>
+    <t>Mean of bottle closure date-time for all rosette bottles included in measurement</t>
+  </si>
+  <si>
+    <t>Mean of ship's latitude when rosette bottles closed</t>
+  </si>
+  <si>
+    <t>Mean of ship's longitude when rosette bottles closed</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1248,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1295,7 +1304,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>169</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
@@ -1316,7 +1325,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>170</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -1337,7 +1346,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
draft of version 2
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6236D34-E0B0-444C-A3E3-132A7882D082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F9108-6054-4F9F-8B52-D237637D36B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33120" yWindow="2895" windowWidth="16860" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="183">
   <si>
     <t>attributeName</t>
   </si>
@@ -586,6 +586,9 @@
   </si>
   <si>
     <t>incubation occurred at 18 degrees C instead of ambient temperature</t>
+  </si>
+  <si>
+    <t>Identifier for incubation type (either ambient or experiemental)</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -645,12 +648,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -682,6 +700,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -965,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A18" sqref="A18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,7 +1285,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1283,6 +1304,18 @@
       <c r="G17" t="s">
         <v>100</v>
       </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1566,7 +1599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCA061C-6977-48E5-9053-BCD9FB4DDE1B}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated data tables, cols, and methods
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F9108-6054-4F9F-8B52-D237637D36B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE8B58D-81A3-419E-8B49-D9A139FC0C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33120" yWindow="2895" windowWidth="16860" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="21084" windowHeight="10584" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="182">
   <si>
     <t>attributeName</t>
   </si>
@@ -132,9 +132,6 @@
     <t>meter</t>
   </si>
   <si>
-    <t>station</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -384,9 +381,6 @@
     <t>Filtered on 0.7 micron filter with 5 micron prefilter</t>
   </si>
   <si>
-    <t>NES-LTER standard station from which sample was collected</t>
-  </si>
-  <si>
     <t>Integer indicating replicate subsample drawn from the same Niskin</t>
   </si>
   <si>
@@ -589,6 +583,9 @@
   </si>
   <si>
     <t>Identifier for incubation type (either ambient or experiemental)</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -668,12 +665,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -685,21 +681,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -988,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,7 +1019,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -1055,7 +1039,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
@@ -1075,7 +1059,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
@@ -1095,7 +1079,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>11</v>
@@ -1115,7 +1099,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>11</v>
@@ -1134,14 +1118,14 @@
       <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="F7" t="s">
-        <v>10</v>
+      <c r="F7" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1154,8 +1138,8 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
-        <v>10</v>
+      <c r="F8" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -1163,10 +1147,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>125</v>
+        <v>158</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -1174,39 +1158,38 @@
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>129</v>
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10"/>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -1214,17 +1197,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -1232,19 +1214,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>127</v>
+        <v>79</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>126</v>
+      <c r="D14" t="s">
+        <v>124</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -1252,17 +1234,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="10"/>
+        <v>88</v>
+      </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -1270,52 +1251,52 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>102</v>
-      </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="17"/>
+      <c r="A18" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1327,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E222AF61-B576-4B64-A4C5-3AFEBBF14AEC}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,254 +1319,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>128</v>
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>171</v>
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>120</v>
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="D12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>161</v>
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>159</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>122</v>
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="D14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1597,9 +1570,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCA061C-6977-48E5-9053-BCD9FB4DDE1B}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1614,427 +1587,379 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
         <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>123</v>
+        <v>76</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="7">
+        <v>80</v>
+      </c>
+      <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="7">
+        <v>80</v>
+      </c>
+      <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="7">
+        <v>80</v>
+      </c>
+      <c r="B7" s="6">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="7">
+        <v>80</v>
+      </c>
+      <c r="B8" s="6">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="7">
+        <v>80</v>
+      </c>
+      <c r="B9" s="6">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>131</v>
+        <v>84</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>132</v>
+        <v>84</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>149</v>
+        <v>75</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>130</v>
+        <v>75</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>133</v>
+        <v>75</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>134</v>
+        <v>75</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <v>0.1</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21">
         <v>15</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23">
         <v>30</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24">
         <v>40</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25">
         <v>50</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26">
         <v>65</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27">
         <v>70</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28">
         <v>75</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29">
         <v>85</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="C29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="C31" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C32" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="10"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C33" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2059,243 +1984,243 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
-        <v>60</v>
-      </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
         <v>62</v>
-      </c>
-      <c r="J2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
         <v>61</v>
       </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>62</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" t="s">
         <v>66</v>
       </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
       <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
         <v>61</v>
       </c>
-      <c r="H4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" t="s">
-        <v>67</v>
-      </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" t="s">
         <v>62</v>
-      </c>
-      <c r="J5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
         <v>69</v>
       </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>70</v>
       </c>
-      <c r="G6" t="s">
-        <v>71</v>
-      </c>
       <c r="H6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
         <v>62</v>
-      </c>
-      <c r="J6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" t="s">
         <v>74</v>
       </c>
-      <c r="F7" t="s">
-        <v>75</v>
-      </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
         <v>62</v>
-      </c>
-      <c r="J7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>163</v>
       </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="G8" t="s">
         <v>164</v>
       </c>
-      <c r="F8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G8" t="s">
-        <v>166</v>
-      </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" t="s">
         <v>62</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2327,90 +2252,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="B11" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2434,53 +2359,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
         <v>151</v>
-      </c>
-      <c r="C2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to v3 change author order
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48B17AF-E7B5-482E-A1FA-1D06834EF087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BAA1FD-13E0-4BDA-A135-ED1259FB4E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
@@ -1284,7 +1284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E222AF61-B576-4B64-A4C5-3AFEBBF14AEC}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12:F14"/>
     </sheetView>
   </sheetViews>
@@ -1947,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FB71B2-251C-4C70-A42B-DE90E8FB59EC}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2022,24 +2022,24 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>59</v>
@@ -2054,24 +2054,24 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
         <v>59</v>
@@ -2202,10 +2202,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{B876B57E-F40C-4019-9902-E3F5F210A4B5}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{BC3EDBC0-671D-451E-BB61-743090D6124F}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{BC3EDBC0-671D-451E-BB61-743090D6124F}"/>
     <hyperlink ref="E7" r:id="rId3" xr:uid="{ABC8AAB7-95D6-4B09-8D74-EC58F97B7FC9}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{B197A09B-50AF-4335-9439-0ADC5614820A}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{C478F55C-B590-48E5-AECF-BCE8DA56F3E8}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{C478F55C-B590-48E5-AECF-BCE8DA56F3E8}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{46C996E6-62E0-4AE9-860A-E9CECA7008F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add POC and methods edits
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BAA1FD-13E0-4BDA-A135-ED1259FB4E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7F5D1A-2B56-4DE0-913C-2604151A9410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
     <sheet name="ColumnHeadersIntegrated" sheetId="2" r:id="rId2"/>
-    <sheet name="CategoricalVariables" sheetId="3" r:id="rId3"/>
-    <sheet name="Personnel" sheetId="4" r:id="rId4"/>
-    <sheet name="Keywords" sheetId="5" r:id="rId5"/>
-    <sheet name="CustomUnits" sheetId="7" r:id="rId6"/>
+    <sheet name="ColumnHeadersPOC" sheetId="8" r:id="rId3"/>
+    <sheet name="CategoricalVariables" sheetId="3" r:id="rId4"/>
+    <sheet name="Personnel" sheetId="4" r:id="rId5"/>
+    <sheet name="Keywords" sheetId="5" r:id="rId6"/>
+    <sheet name="CustomUnits" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="184">
   <si>
     <t>attributeName</t>
   </si>
@@ -574,13 +575,31 @@
   </si>
   <si>
     <t>station</t>
+  </si>
+  <si>
+    <t>vol_filt_L</t>
+  </si>
+  <si>
+    <t>POC_ug_L</t>
+  </si>
+  <si>
+    <t>microgramsPerLiter</t>
+  </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>Volume of seawater filtered to obtain POC sample</t>
+  </si>
+  <si>
+    <t>Particulate organic carbon http://vocab.nerc.ac.uk/collection/P09/current/POCP/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,6 +642,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -632,27 +658,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -681,10 +692,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -969,7 +978,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,7 +1094,7 @@
       <c r="A6" t="s">
         <v>177</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>176</v>
       </c>
       <c r="C6" t="s">
@@ -1245,7 +1254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1262,17 +1271,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1285,7 +1294,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:F14"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,7 +1407,7 @@
       <c r="A6" t="s">
         <v>177</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>176</v>
       </c>
       <c r="C6" t="s">
@@ -1545,11 +1554,323 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4CB2F6-D54E-4E01-A2DD-6C9548550709}">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="37.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCA061C-6977-48E5-9053-BCD9FB4DDE1B}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1943,11 +2264,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FB71B2-251C-4C70-A42B-DE90E8FB59EC}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -2212,7 +2533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D588F7-ACAE-4AAB-8E67-973953C0CDDF}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -2319,7 +2640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B88C0FB-B81B-4182-8D44-742C6584AC87}">
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix header and missing value code
</commit_message>
<xml_diff>
--- a/npp-transect-info.xlsx
+++ b/npp-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-npp-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED31FE09-368A-4263-81B0-B587312AB4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B8212E-F52B-4419-A59A-76543F93CB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersDiscrete" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="184">
   <si>
     <t>attributeName</t>
   </si>
@@ -580,9 +580,6 @@
     <t>vol_filt_L</t>
   </si>
   <si>
-    <t>POC_ug_L</t>
-  </si>
-  <si>
     <t>microgramsPerLiter</t>
   </si>
   <si>
@@ -592,7 +589,10 @@
     <t>Volume of seawater filtered to obtain POC sample</t>
   </si>
   <si>
-    <t>Particulate organic carbon http://vocab.nerc.ac.uk/collection/P01/current/CORGCAP1/</t>
+    <t>Particulate organic carbon in micrograms per liter http://vocab.nerc.ac.uk/collection/P01/current/CORGCAP1/</t>
+  </si>
+  <si>
+    <t>POC_microg_perL</t>
   </si>
 </sst>
 </file>
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E222AF61-B576-4B64-A4C5-3AFEBBF14AEC}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1464,6 +1464,12 @@
       <c r="D9" t="s">
         <v>140</v>
       </c>
+      <c r="F9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1474,6 +1480,12 @@
       </c>
       <c r="C10" s="5" t="s">
         <v>85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1557,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4CB2F6-D54E-4E01-A2DD-6C9548550709}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1746,27 +1758,27 @@
         <v>178</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>